<commit_message>
debug of deleting identical anchors
</commit_message>
<xml_diff>
--- a/potential_customer.xlsx
+++ b/potential_customer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL17"/>
+  <dimension ref="A1:AL14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -622,58 +622,58 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G2" t="n">
         <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I2" t="n">
         <v>2</v>
       </c>
       <c r="J2" t="n">
-        <v>34516</v>
+        <v>1494</v>
       </c>
       <c r="K2" t="n">
-        <v>1527</v>
+        <v>706</v>
       </c>
       <c r="L2" t="n">
-        <v>32989</v>
+        <v>788</v>
       </c>
       <c r="M2" t="n">
-        <v>0.526</v>
+        <v>1.674</v>
       </c>
       <c r="N2" t="n">
-        <v>1268</v>
+        <v>1305</v>
       </c>
       <c r="O2" t="n">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="P2" t="n">
-        <v>0.355</v>
+        <v>3</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.044</v>
+        <v>0.473</v>
       </c>
       <c r="R2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
@@ -688,7 +688,7 @@
         <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2" t="n">
         <v>0</v>
@@ -697,16 +697,16 @@
         <v>0</v>
       </c>
       <c r="Z2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB2" t="n">
         <v>0</v>
       </c>
       <c r="AC2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
@@ -718,13 +718,13 @@
         <v>0</v>
       </c>
       <c r="AG2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH2" t="n">
         <v>0</v>
       </c>
       <c r="AI2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ2" t="n">
         <v>0</v>
@@ -733,63 +733,63 @@
         <v>0</v>
       </c>
       <c r="AL2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>8248</v>
+        <v>124</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3" t="n">
         <v>34516</v>
       </c>
       <c r="K3" t="n">
-        <v>2045</v>
+        <v>1527</v>
       </c>
       <c r="L3" t="n">
-        <v>32471</v>
+        <v>32989</v>
       </c>
       <c r="M3" t="n">
-        <v>0.59</v>
+        <v>0.526</v>
       </c>
       <c r="N3" t="n">
-        <v>4081</v>
+        <v>1268</v>
       </c>
       <c r="O3" t="n">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="P3" t="n">
-        <v>0.421</v>
+        <v>0.355</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.059</v>
+        <v>0.044</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -798,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
         <v>0</v>
@@ -813,16 +813,16 @@
         <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB3" t="n">
         <v>0</v>
       </c>
       <c r="AC3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -831,7 +831,7 @@
         <v>0</v>
       </c>
       <c r="AF3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG3" t="n">
         <v>0</v>
@@ -854,13 +854,13 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>1541</v>
+        <v>63</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -869,40 +869,40 @@
         <v>4</v>
       </c>
       <c r="F4" t="n">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H4" t="n">
+        <v>4</v>
+      </c>
+      <c r="I4" t="n">
         <v>2</v>
       </c>
-      <c r="I4" t="n">
-        <v>4</v>
-      </c>
       <c r="J4" t="n">
-        <v>6784</v>
+        <v>23957</v>
       </c>
       <c r="K4" t="n">
-        <v>891</v>
+        <v>2102</v>
       </c>
       <c r="L4" t="n">
-        <v>5893</v>
+        <v>21855</v>
       </c>
       <c r="M4" t="n">
-        <v>1.047</v>
+        <v>0.997</v>
       </c>
       <c r="N4" t="n">
-        <v>1900</v>
+        <v>1276</v>
       </c>
       <c r="O4" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P4" t="n">
-        <v>0.556</v>
+        <v>0.733</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.131</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>
@@ -911,13 +911,13 @@
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4" t="n">
         <v>0</v>
@@ -926,25 +926,25 @@
         <v>0</v>
       </c>
       <c r="Y4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4" t="n">
         <v>0</v>
       </c>
       <c r="AA4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB4" t="n">
         <v>0</v>
       </c>
       <c r="AC4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
       </c>
       <c r="AE4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF4" t="n">
         <v>0</v>
@@ -970,64 +970,64 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>1151</v>
+        <v>209</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="G5" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H5" t="n">
         <v>3</v>
       </c>
       <c r="I5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>1467</v>
+        <v>24407</v>
       </c>
       <c r="K5" t="n">
-        <v>896</v>
+        <v>2395</v>
       </c>
       <c r="L5" t="n">
-        <v>571</v>
+        <v>22012</v>
       </c>
       <c r="M5" t="n">
-        <v>0.6919999999999999</v>
+        <v>1.071</v>
       </c>
       <c r="N5" t="n">
-        <v>1731</v>
+        <v>2311</v>
       </c>
       <c r="O5" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="P5" t="n">
-        <v>0.5</v>
+        <v>0.714</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.611</v>
+        <v>0.098</v>
       </c>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5" t="n">
         <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5" t="n">
         <v>0</v>
@@ -1042,10 +1042,10 @@
         <v>0</v>
       </c>
       <c r="Y5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA5" t="n">
         <v>0</v>
@@ -1054,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="AC5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -1066,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="AG5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH5" t="n">
         <v>0</v>
@@ -1086,55 +1086,55 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>3902</v>
+        <v>8189</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>36</v>
       </c>
       <c r="G6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
         <v>3</v>
       </c>
       <c r="I6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J6" t="n">
-        <v>27876</v>
+        <v>1572</v>
       </c>
       <c r="K6" t="n">
-        <v>557</v>
+        <v>985</v>
       </c>
       <c r="L6" t="n">
-        <v>27319</v>
+        <v>587</v>
       </c>
       <c r="M6" t="n">
-        <v>0.768</v>
+        <v>0.745</v>
       </c>
       <c r="N6" t="n">
-        <v>4654</v>
+        <v>4148</v>
       </c>
       <c r="O6" t="n">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="P6" t="n">
-        <v>0.66</v>
+        <v>0.862</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02</v>
+        <v>0.627</v>
       </c>
       <c r="R6" t="n">
         <v>0</v>
@@ -1146,13 +1146,13 @@
         <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" t="n">
         <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X6" t="n">
         <v>0</v>
@@ -1170,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="AC6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
@@ -1182,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="AG6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH6" t="n">
         <v>0</v>
@@ -1202,55 +1202,55 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>7931</v>
+        <v>260</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
       </c>
       <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>22</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
         <v>3</v>
       </c>
-      <c r="F7" t="n">
-        <v>37</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>3</v>
-      </c>
-      <c r="I7" t="n">
-        <v>2</v>
-      </c>
       <c r="J7" t="n">
-        <v>2449</v>
+        <v>34516</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>1652</v>
       </c>
       <c r="L7" t="n">
-        <v>2449</v>
+        <v>32864</v>
       </c>
       <c r="M7" t="n">
-        <v>0.706</v>
+        <v>0.854</v>
       </c>
       <c r="N7" t="n">
-        <v>5497</v>
+        <v>1283</v>
       </c>
       <c r="O7" t="n">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="P7" t="n">
-        <v>0.63</v>
+        <v>1.294</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>0.048</v>
       </c>
       <c r="R7" t="n">
         <v>1</v>
@@ -1274,7 +1274,7 @@
         <v>0</v>
       </c>
       <c r="Y7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z7" t="n">
         <v>0</v>
@@ -1283,19 +1283,19 @@
         <v>0</v>
       </c>
       <c r="AB7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC7" t="n">
         <v>0</v>
       </c>
       <c r="AD7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE7" t="n">
         <v>0</v>
       </c>
       <c r="AF7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG7" t="n">
         <v>0</v>
@@ -1318,55 +1318,55 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>163</v>
+        <v>258</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G8" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H8" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I8" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>3482</v>
+        <v>3540</v>
       </c>
       <c r="K8" t="n">
-        <v>2114</v>
+        <v>849</v>
       </c>
       <c r="L8" t="n">
-        <v>1368</v>
+        <v>2691</v>
       </c>
       <c r="M8" t="n">
-        <v>0.508</v>
+        <v>0.456</v>
       </c>
       <c r="N8" t="n">
-        <v>1039</v>
+        <v>1321</v>
       </c>
       <c r="O8" t="n">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="P8" t="n">
-        <v>0.263</v>
+        <v>0.75</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.607</v>
+        <v>0.24</v>
       </c>
       <c r="R8" t="n">
         <v>0</v>
@@ -1384,19 +1384,19 @@
         <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z8" t="n">
         <v>0</v>
       </c>
       <c r="AA8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB8" t="n">
         <v>0</v>
@@ -1405,7 +1405,7 @@
         <v>0</v>
       </c>
       <c r="AD8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE8" t="n">
         <v>0</v>
@@ -1414,7 +1414,7 @@
         <v>0</v>
       </c>
       <c r="AG8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH8" t="n">
         <v>0</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>374</v>
+        <v>152</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -1449,40 +1449,40 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="G9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H9" t="n">
         <v>2</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J9" t="n">
-        <v>2569</v>
+        <v>18386</v>
       </c>
       <c r="K9" t="n">
-        <v>1403</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>1166</v>
+        <v>18386</v>
       </c>
       <c r="M9" t="n">
-        <v>0.886</v>
+        <v>0.868</v>
       </c>
       <c r="N9" t="n">
-        <v>1456</v>
+        <v>1298</v>
       </c>
       <c r="O9" t="n">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="P9" t="n">
-        <v>0.444</v>
+        <v>0.571</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.546</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
         <v>0</v>
@@ -1491,10 +1491,10 @@
         <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V9" t="n">
         <v>0</v>
@@ -1521,7 +1521,7 @@
         <v>0</v>
       </c>
       <c r="AD9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE9" t="n">
         <v>0</v>
@@ -1530,13 +1530,13 @@
         <v>0</v>
       </c>
       <c r="AG9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH9" t="n">
         <v>0</v>
       </c>
       <c r="AI9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ9" t="n">
         <v>0</v>
@@ -1545,60 +1545,60 @@
         <v>0</v>
       </c>
       <c r="AL9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>3428</v>
+        <v>8248</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
         <v>3</v>
       </c>
       <c r="J10" t="n">
-        <v>6245</v>
+        <v>34516</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>2045</v>
       </c>
       <c r="L10" t="n">
-        <v>6245</v>
+        <v>32471</v>
       </c>
       <c r="M10" t="n">
-        <v>0.554</v>
+        <v>0.59</v>
       </c>
       <c r="N10" t="n">
-        <v>2521</v>
+        <v>4081</v>
       </c>
       <c r="O10" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="P10" t="n">
-        <v>0.667</v>
+        <v>0.421</v>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>0.059</v>
       </c>
       <c r="R10" t="n">
         <v>0</v>
@@ -1610,13 +1610,13 @@
         <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10" t="n">
         <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X10" t="n">
         <v>0</v>
@@ -1625,13 +1625,13 @@
         <v>0</v>
       </c>
       <c r="Z10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA10" t="n">
         <v>0</v>
       </c>
       <c r="AB10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC10" t="n">
         <v>0</v>
@@ -1643,16 +1643,16 @@
         <v>0</v>
       </c>
       <c r="AF10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH10" t="n">
         <v>0</v>
       </c>
       <c r="AI10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ10" t="n">
         <v>0</v>
@@ -1661,63 +1661,63 @@
         <v>0</v>
       </c>
       <c r="AL10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>2136</v>
+        <v>7989</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
         <v>3</v>
       </c>
       <c r="J11" t="n">
-        <v>5464</v>
+        <v>7452</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>1656</v>
       </c>
       <c r="L11" t="n">
-        <v>5464</v>
+        <v>5796</v>
       </c>
       <c r="M11" t="n">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="N11" t="n">
-        <v>2473</v>
+        <v>3339</v>
       </c>
       <c r="O11" t="n">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="P11" t="n">
-        <v>0.484</v>
+        <v>0.962</v>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>0.222</v>
       </c>
       <c r="R11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11" t="n">
         <v>0</v>
@@ -1735,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="X11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y11" t="n">
         <v>0</v>
@@ -1744,16 +1744,16 @@
         <v>0</v>
       </c>
       <c r="AA11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC11" t="n">
         <v>0</v>
       </c>
       <c r="AD11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE11" t="n">
         <v>0</v>
@@ -1765,7 +1765,7 @@
         <v>0</v>
       </c>
       <c r="AH11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI11" t="n">
         <v>1</v>
@@ -1782,25 +1782,25 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>1935</v>
+        <v>3428</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H12" t="n">
         <v>4</v>
@@ -1809,25 +1809,25 @@
         <v>3</v>
       </c>
       <c r="J12" t="n">
-        <v>19214</v>
+        <v>6245</v>
       </c>
       <c r="K12" t="n">
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>19214</v>
+        <v>6245</v>
       </c>
       <c r="M12" t="n">
-        <v>0.998</v>
+        <v>0.554</v>
       </c>
       <c r="N12" t="n">
-        <v>3407</v>
+        <v>2521</v>
       </c>
       <c r="O12" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P12" t="n">
-        <v>1.136</v>
+        <v>0.667</v>
       </c>
       <c r="Q12" t="n">
         <v>0</v>
@@ -1839,7 +1839,7 @@
         <v>0</v>
       </c>
       <c r="T12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U12" t="n">
         <v>0</v>
@@ -1848,7 +1848,7 @@
         <v>0</v>
       </c>
       <c r="W12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X12" t="n">
         <v>0</v>
@@ -1857,13 +1857,13 @@
         <v>0</v>
       </c>
       <c r="Z12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA12" t="n">
         <v>0</v>
       </c>
       <c r="AB12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC12" t="n">
         <v>0</v>
@@ -1875,10 +1875,10 @@
         <v>0</v>
       </c>
       <c r="AF12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH12" t="n">
         <v>0</v>
@@ -1898,55 +1898,55 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>113</v>
+        <v>2136</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="G13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H13" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J13" t="n">
-        <v>1494</v>
+        <v>5464</v>
       </c>
       <c r="K13" t="n">
-        <v>706</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>788</v>
+        <v>5464</v>
       </c>
       <c r="M13" t="n">
-        <v>1.674</v>
+        <v>0.7</v>
       </c>
       <c r="N13" t="n">
-        <v>1305</v>
+        <v>2473</v>
       </c>
       <c r="O13" t="n">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="P13" t="n">
-        <v>3</v>
+        <v>0.484</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.473</v>
+        <v>0</v>
       </c>
       <c r="R13" t="n">
         <v>0</v>
@@ -1964,19 +1964,19 @@
         <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y13" t="n">
         <v>0</v>
       </c>
       <c r="Z13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB13" t="n">
         <v>0</v>
@@ -1994,10 +1994,10 @@
         <v>0</v>
       </c>
       <c r="AG13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI13" t="n">
         <v>1</v>
@@ -2014,7 +2014,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>63</v>
+        <v>1935</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -2026,43 +2026,43 @@
         <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G14" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H14" t="n">
         <v>4</v>
       </c>
       <c r="I14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J14" t="n">
-        <v>23957</v>
+        <v>19214</v>
       </c>
       <c r="K14" t="n">
-        <v>2102</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>21855</v>
+        <v>19214</v>
       </c>
       <c r="M14" t="n">
-        <v>0.997</v>
+        <v>0.998</v>
       </c>
       <c r="N14" t="n">
-        <v>1276</v>
+        <v>3407</v>
       </c>
       <c r="O14" t="n">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="P14" t="n">
-        <v>0.733</v>
+        <v>1.136</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.08799999999999999</v>
+        <v>0</v>
       </c>
       <c r="R14" t="n">
         <v>0</v>
@@ -2071,13 +2071,13 @@
         <v>0</v>
       </c>
       <c r="T14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14" t="n">
         <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W14" t="n">
         <v>0</v>
@@ -2089,16 +2089,16 @@
         <v>0</v>
       </c>
       <c r="Z14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB14" t="n">
         <v>0</v>
       </c>
       <c r="AC14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD14" t="n">
         <v>0</v>
@@ -2107,7 +2107,7 @@
         <v>0</v>
       </c>
       <c r="AF14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG14" t="n">
         <v>0</v>
@@ -2126,354 +2126,6 @@
       </c>
       <c r="AL14" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>260</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>36</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" t="n">
-        <v>2</v>
-      </c>
-      <c r="F15" t="n">
-        <v>22</v>
-      </c>
-      <c r="G15" t="n">
-        <v>2</v>
-      </c>
-      <c r="H15" t="n">
-        <v>2</v>
-      </c>
-      <c r="I15" t="n">
-        <v>3</v>
-      </c>
-      <c r="J15" t="n">
-        <v>34516</v>
-      </c>
-      <c r="K15" t="n">
-        <v>1652</v>
-      </c>
-      <c r="L15" t="n">
-        <v>32864</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0.854</v>
-      </c>
-      <c r="N15" t="n">
-        <v>1283</v>
-      </c>
-      <c r="O15" t="n">
-        <v>39</v>
-      </c>
-      <c r="P15" t="n">
-        <v>1.294</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>0.048</v>
-      </c>
-      <c r="R15" t="n">
-        <v>1</v>
-      </c>
-      <c r="S15" t="n">
-        <v>0</v>
-      </c>
-      <c r="T15" t="n">
-        <v>0</v>
-      </c>
-      <c r="U15" t="n">
-        <v>0</v>
-      </c>
-      <c r="V15" t="n">
-        <v>0</v>
-      </c>
-      <c r="W15" t="n">
-        <v>0</v>
-      </c>
-      <c r="X15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>258</v>
-      </c>
-      <c r="B16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" t="n">
-        <v>45</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" t="n">
-        <v>2</v>
-      </c>
-      <c r="F16" t="n">
-        <v>35</v>
-      </c>
-      <c r="G16" t="n">
-        <v>2</v>
-      </c>
-      <c r="H16" t="n">
-        <v>3</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>3540</v>
-      </c>
-      <c r="K16" t="n">
-        <v>849</v>
-      </c>
-      <c r="L16" t="n">
-        <v>2691</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0.456</v>
-      </c>
-      <c r="N16" t="n">
-        <v>1321</v>
-      </c>
-      <c r="O16" t="n">
-        <v>28</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="R16" t="n">
-        <v>0</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0</v>
-      </c>
-      <c r="T16" t="n">
-        <v>0</v>
-      </c>
-      <c r="U16" t="n">
-        <v>0</v>
-      </c>
-      <c r="V16" t="n">
-        <v>0</v>
-      </c>
-      <c r="W16" t="n">
-        <v>1</v>
-      </c>
-      <c r="X16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>152</v>
-      </c>
-      <c r="B17" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" t="n">
-        <v>50</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" t="n">
-        <v>31</v>
-      </c>
-      <c r="G17" t="n">
-        <v>2</v>
-      </c>
-      <c r="H17" t="n">
-        <v>2</v>
-      </c>
-      <c r="I17" t="n">
-        <v>3</v>
-      </c>
-      <c r="J17" t="n">
-        <v>18386</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" t="n">
-        <v>18386</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0.868</v>
-      </c>
-      <c r="N17" t="n">
-        <v>1298</v>
-      </c>
-      <c r="O17" t="n">
-        <v>22</v>
-      </c>
-      <c r="P17" t="n">
-        <v>0.571</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>0</v>
-      </c>
-      <c r="R17" t="n">
-        <v>0</v>
-      </c>
-      <c r="S17" t="n">
-        <v>0</v>
-      </c>
-      <c r="T17" t="n">
-        <v>1</v>
-      </c>
-      <c r="U17" t="n">
-        <v>0</v>
-      </c>
-      <c r="V17" t="n">
-        <v>0</v>
-      </c>
-      <c r="W17" t="n">
-        <v>0</v>
-      </c>
-      <c r="X17" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y17" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL17" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>